<commit_message>
231031 - Inversionistas Responsive
</commit_message>
<xml_diff>
--- a/data/inversionistas_input.xlsx
+++ b/data/inversionistas_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar Israel Cano\workspace\okysoft\Planigrupo\Sitio Web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA8C05E-800F-4155-BEB9-FBF5083C8073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22862F88-4554-40F9-8DED-F59B6FB7C3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4995" yWindow="885" windowWidth="20610" windowHeight="14160" xr2:uid="{562CD49C-6CFB-B54D-B1A7-F1CF16783197}"/>
+    <workbookView xWindow="1125" yWindow="615" windowWidth="20610" windowHeight="14160" xr2:uid="{562CD49C-6CFB-B54D-B1A7-F1CF16783197}"/>
   </bookViews>
   <sheets>
     <sheet name="Res Fin 2do trim 2023" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
20231113 - Fixed Property Detail JSON
</commit_message>
<xml_diff>
--- a/data/inversionistas_input.xlsx
+++ b/data/inversionistas_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar Israel Cano\workspace\okysoft\Planigrupo\Sitio Web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22862F88-4554-40F9-8DED-F59B6FB7C3C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF0733-A799-44B1-B510-4D321BC5ADCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="615" windowWidth="20610" windowHeight="14160" xr2:uid="{562CD49C-6CFB-B54D-B1A7-F1CF16783197}"/>
+    <workbookView xWindow="4005" yWindow="2235" windowWidth="20610" windowHeight="12555" xr2:uid="{562CD49C-6CFB-B54D-B1A7-F1CF16783197}"/>
   </bookViews>
   <sheets>
     <sheet name="Res Fin 2do trim 2023" sheetId="1" r:id="rId1"/>
@@ -1226,7 +1226,7 @@
     <t>59.6%</t>
   </si>
   <si>
-    <t>9.40%</t>
+    <t>RAMIRO LA PERSONA</t>
   </si>
 </sst>
 </file>
@@ -1683,7 +1683,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
20231113 - Fixed Compormise Text
</commit_message>
<xml_diff>
--- a/data/inversionistas_input.xlsx
+++ b/data/inversionistas_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edgar Israel Cano\workspace\okysoft\Planigrupo\Sitio Web\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABFF0733-A799-44B1-B510-4D321BC5ADCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D7A218-18BB-4178-A419-07E5436CE2D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4005" yWindow="2235" windowWidth="20610" windowHeight="12555" xr2:uid="{562CD49C-6CFB-B54D-B1A7-F1CF16783197}"/>
   </bookViews>
@@ -1226,7 +1226,7 @@
     <t>59.6%</t>
   </si>
   <si>
-    <t>RAMIRO LA PERSONA</t>
+    <t>94.50%</t>
   </si>
 </sst>
 </file>
@@ -1683,7 +1683,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>